<commit_message>
[Shreya]Add: Added Flipkart Process and refactored Business object
</commit_message>
<xml_diff>
--- a/flipkart/FlipkartData.xlsx
+++ b/flipkart/FlipkartData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shreya\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shreya\Desktop\ASSIGNMENTS\FlipkartBluePrism\FlipkartBluePrism\flipkart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A920763B-02C2-4CBD-A16F-E215C6F57F56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1C89EC-757A-4CAC-8540-DD40043915BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{FCED1DB9-3D17-4CB0-8CA1-4C4A5435F909}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FCED1DB9-3D17-4CB0-8CA1-4C4A5435F909}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Apple iPhone 11 (White, 64 GB) (Includes EarPods, Power Adapter)</t>
+  </si>
+  <si>
+    <t>Colour</t>
   </si>
 </sst>
 </file>
@@ -394,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74A4AE62-029D-4567-A1F4-580C4E800C0C}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -407,7 +410,7 @@
     <col min="3" max="3" width="6.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -417,8 +420,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -429,7 +435,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -440,7 +446,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -451,7 +457,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -462,7 +468,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -473,7 +479,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -484,7 +490,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -495,7 +501,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -506,7 +512,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -517,7 +523,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>

</xml_diff>